<commit_message>
vault backup: 2024-10-10 11:43:53
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/Caceres_Ivan_S1.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/Caceres_Ivan_S1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivaaan\Desktop\git\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C29779D-5686-4BC5-BC4B-9B4FFC0A5851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497EF316-17DC-4E39-B27B-CC7B8D59B2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF03DFFC-242D-4D34-A20F-21711E55E767}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DF03DFFC-242D-4D34-A20F-21711E55E767}"/>
   </bookViews>
   <sheets>
     <sheet name="PREGUNTA 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -303,9 +303,9 @@
   <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="0.000%"/>
-    <numFmt numFmtId="169" formatCode="0.0000%"/>
-    <numFmt numFmtId="170" formatCode="_ &quot;$&quot;* #,##0.0000_ ;_ &quot;$&quot;* \-#,##0.0000_ ;_ &quot;$&quot;* &quot;-&quot;????_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="_ &quot;$&quot;* #,##0.0000_ ;_ &quot;$&quot;* \-#,##0.0000_ ;_ &quot;$&quot;* &quot;-&quot;????_ ;_ @_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -470,18 +470,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,53 +483,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -546,63 +571,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -2385,7 +2383,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE11E083-4EBD-46FC-9081-E4D34EACDB7F}" name="TablaDinámica2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="AÑO">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE11E083-4EBD-46FC-9081-E4D34EACDB7F}" name="TablaDinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="AÑO">
   <location ref="E6:H33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -2884,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C0A6B6-3D4C-4BB0-B288-1456ACA69B51}">
   <dimension ref="A3:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2899,174 +2897,174 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="2" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15">
+      <c r="C9" s="60"/>
+      <c r="D9" s="11">
         <v>85000000</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="8">
         <f>D9</f>
         <v>85000000</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6">
+      <c r="C10" s="52"/>
+      <c r="D10" s="61">
         <v>0.12</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="9">
         <f>J9*$D$14</f>
         <v>10668248.849999992</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="10">
         <f>$D$15</f>
         <v>20997750.909768987</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <f>H10-G10</f>
         <v>10329502.059768995</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <f>J9-I10</f>
         <v>74670497.94023101</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="F11" s="2">
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="54"/>
+      <c r="F11" s="1">
         <v>2</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="9">
         <f t="shared" ref="G11:G15" si="0">J10*$D$14</f>
         <v>9371805.3385858387</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="10">
         <f t="shared" ref="H11:H15" si="1">$D$15</f>
         <v>20997750.909768987</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <f t="shared" ref="I11:I15" si="2">H11-G11</f>
         <v>11625945.571183149</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <f t="shared" ref="J11:J15" si="3">J10-I11</f>
         <v>63044552.369047865</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="7"/>
-      <c r="F12" s="2">
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="54"/>
+      <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <f t="shared" si="0"/>
         <v>7912646.7448218735</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="10">
         <f t="shared" si="1"/>
         <v>20997750.909768987</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <f t="shared" si="2"/>
         <v>13085104.164947115</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <f t="shared" si="3"/>
         <v>49959448.20410075</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="8">
+      <c r="C13" s="55"/>
+      <c r="D13" s="5">
         <v>6</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="13">
         <v>4</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="14">
         <f t="shared" si="0"/>
         <v>6270350.8923533177</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="15">
         <f t="shared" si="1"/>
         <v>20997750.909768987</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="13">
         <f t="shared" si="2"/>
         <v>14727400.017415669</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="16">
         <f t="shared" si="3"/>
         <v>35232048.186685085</v>
       </c>
@@ -3075,204 +3073,204 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="9">
+      <c r="C14" s="55"/>
+      <c r="D14" s="6">
         <f>POWER(1+D10/4,4)-1</f>
         <v>0.12550880999999992</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>5</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="9">
         <f t="shared" si="0"/>
         <v>4421932.4417735003</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="10">
         <f t="shared" si="1"/>
         <v>20997750.909768987</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <f t="shared" si="2"/>
         <v>16575818.467995487</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="8">
         <f t="shared" si="3"/>
         <v>18656229.718689598</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="10">
+      <c r="C15" s="55"/>
+      <c r="D15" s="7">
         <f>-PMT(D14,D13,D9)</f>
         <v>20997750.909768987</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>6</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="9">
         <f t="shared" si="0"/>
         <v>2341521.1910793646</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="10">
         <f t="shared" si="1"/>
         <v>20997750.909768987</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <f t="shared" si="2"/>
         <v>18656229.718689624</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="22" t="s">
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="11">
+      <c r="C18" s="55"/>
+      <c r="D18" s="8">
         <f>J13</f>
         <v>35232048.186685085</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="8">
         <f>D18</f>
         <v>35232048.186685085</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="26">
+      <c r="C19" s="52"/>
+      <c r="D19" s="59">
         <v>0.05</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="9">
         <f>J18*$D$23</f>
         <v>1802538.4514914935</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="10">
         <f>$D$24</f>
         <v>9962684.9212262407</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <f>H19-G19</f>
         <v>8160146.469734747</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="8">
         <f>J18-I19</f>
         <v>27071901.716950338</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="1"/>
-      <c r="F20" s="2">
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="55"/>
+      <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="9">
         <f t="shared" ref="G20:G22" si="4">J19*$D$23</f>
         <v>1385049.8711069368</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="10">
         <f t="shared" ref="H20:H22" si="5">$D$24</f>
         <v>9962684.9212262407</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <f t="shared" ref="I20:I22" si="6">H20-G20</f>
         <v>8577635.0501193032</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="8">
         <f t="shared" ref="J20:J22" si="7">J19-I20</f>
         <v>18494266.666831035</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="1"/>
-      <c r="F21" s="2">
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="55"/>
+      <c r="F21" s="1">
         <v>3</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="9">
         <f t="shared" si="4"/>
         <v>946201.78260595573</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="10">
         <f t="shared" si="5"/>
         <v>9962684.9212262407</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <f t="shared" si="6"/>
         <v>9016483.1386202853</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="8">
         <f t="shared" si="7"/>
         <v>9477783.5282107498</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2">
+      <c r="C22" s="55"/>
+      <c r="D22" s="1">
         <v>4</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="13">
         <v>4</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="14">
         <f t="shared" si="4"/>
         <v>484901.39301549346</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="15">
         <f t="shared" si="5"/>
         <v>9962684.9212262407</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="13">
         <f t="shared" si="6"/>
         <v>9477783.528210748</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="16">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3281,531 +3279,504 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="27">
+      <c r="C23" s="48"/>
+      <c r="D23" s="19">
         <f>POWER(1+D19/12,12)-1</f>
         <v>5.116189788173342E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="13">
+      <c r="C24" s="55"/>
+      <c r="D24" s="10">
         <f>-PMT(D23,D22,D18)</f>
         <v>9962684.9212262407</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="28">
+      <c r="C27" s="48"/>
+      <c r="D27" s="20">
         <v>0.03</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="10">
         <f>$D$15</f>
         <v>20997750.909768987</v>
       </c>
-      <c r="D30" s="13">
-        <f>-PV($D$27,B30,,C30)</f>
+      <c r="D30" s="10">
+        <f t="shared" ref="D30:D37" si="8">-PV($D$27,B30,,C30)</f>
         <v>20386165.931814551</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="33">
+      <c r="G30" s="49"/>
+      <c r="H30" s="50">
         <f>SUM(D30:D37)</f>
         <v>110953407.68925402</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>2</v>
       </c>
-      <c r="C31" s="13">
-        <f t="shared" ref="C31:C33" si="8">$D$15</f>
+      <c r="C31" s="10">
+        <f t="shared" ref="C31:C33" si="9">$D$15</f>
         <v>20997750.909768987</v>
       </c>
-      <c r="D31" s="13">
-        <f>-PV($D$27,B31,,C31)</f>
+      <c r="D31" s="10">
+        <f t="shared" si="8"/>
         <v>19792394.108557817</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="34"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="51"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>3</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="10">
+        <f t="shared" si="9"/>
+        <v>20997750.909768987</v>
+      </c>
+      <c r="D32" s="10">
         <f t="shared" si="8"/>
+        <v>19215916.610250305</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <v>4</v>
+      </c>
+      <c r="C33" s="10">
+        <f t="shared" si="9"/>
         <v>20997750.909768987</v>
       </c>
-      <c r="D32" s="13">
-        <f>-PV($D$27,B32,,C32)</f>
-        <v>19215916.610250305</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="13">
+      <c r="D33" s="10">
         <f t="shared" si="8"/>
-        <v>20997750.909768987</v>
-      </c>
-      <c r="D33" s="13">
-        <f>-PV($D$27,B33,,C33)</f>
         <v>18656229.71868962</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>5</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="10">
         <f>$D$24</f>
         <v>9962684.9212262407</v>
       </c>
-      <c r="D34" s="13">
-        <f>-PV($D$27,B34,,C34)</f>
+      <c r="D34" s="10">
+        <f t="shared" si="8"/>
         <v>8593899.529101409</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>6</v>
       </c>
-      <c r="C35" s="13">
-        <f t="shared" ref="C35:C37" si="9">$D$24</f>
+      <c r="C35" s="10">
+        <f t="shared" ref="C35:C37" si="10">$D$24</f>
         <v>9962684.9212262407</v>
       </c>
-      <c r="D35" s="13">
-        <f>-PV($D$27,B35,,C35)</f>
+      <c r="D35" s="10">
+        <f t="shared" si="8"/>
         <v>8343591.7758266106</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>7</v>
       </c>
-      <c r="C36" s="13">
-        <f t="shared" si="9"/>
+      <c r="C36" s="10">
+        <f t="shared" si="10"/>
         <v>9962684.9212262407</v>
       </c>
-      <c r="D36" s="13">
-        <f>-PV($D$27,B36,,C36)</f>
+      <c r="D36" s="10">
+        <f t="shared" si="8"/>
         <v>8100574.5396374855</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>8</v>
       </c>
-      <c r="C37" s="13">
-        <f t="shared" si="9"/>
+      <c r="C37" s="10">
+        <f t="shared" si="10"/>
         <v>9962684.9212262407</v>
       </c>
-      <c r="D37" s="13">
-        <f>-PV($D$27,B37,,C37)</f>
+      <c r="D37" s="10">
+        <f t="shared" si="8"/>
         <v>7864635.4753761999</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="G40" s="1" t="s">
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="G40" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="50">
+      <c r="H40" s="55"/>
+      <c r="I40" s="35">
         <v>5.116189788173342E-2</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="35">
+      <c r="C41" s="55"/>
+      <c r="D41" s="4">
         <v>0.01</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="13">
+      <c r="H41" s="55"/>
+      <c r="I41" s="10">
         <f>-PMT(I40,4,J43)</f>
         <v>10367209.879394561</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="8">
+      <c r="C42" s="55"/>
+      <c r="D42" s="5">
         <v>4</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F42" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="42" t="s">
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="36">
+      <c r="C43" s="55"/>
+      <c r="D43" s="23">
         <f>J13</f>
         <v>35232048.186685085</v>
       </c>
-      <c r="F43" s="42" t="s">
+      <c r="F43" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G43" s="42" t="s">
+      <c r="G43" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H43" s="42" t="s">
+      <c r="H43" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="42" t="s">
+      <c r="I43" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="J43" s="43">
+      <c r="J43" s="28">
         <f>D47</f>
         <v>36662610.623577729</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="37">
+      <c r="C44" s="55"/>
+      <c r="D44" s="21">
         <f>-FV(D41,D42,,D43)</f>
         <v>36662610.623577729</v>
       </c>
-      <c r="F44" s="42">
+      <c r="F44" s="27">
         <v>1</v>
       </c>
-      <c r="G44" s="44">
+      <c r="G44" s="29">
         <f>J43*$I$40</f>
         <v>1875728.7408012387</v>
       </c>
-      <c r="H44" s="43">
+      <c r="H44" s="28">
         <f>$I$41</f>
         <v>10367209.879394561</v>
       </c>
-      <c r="I44" s="42">
+      <c r="I44" s="27">
         <f>H44-G44</f>
         <v>8491481.1385933217</v>
       </c>
-      <c r="J44" s="45">
+      <c r="J44" s="30">
         <f>J43-I44</f>
         <v>28171129.484984405</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="36">
+      <c r="C45" s="55"/>
+      <c r="D45" s="23">
         <f>D44-D43</f>
         <v>1430562.4368926436</v>
       </c>
-      <c r="F45" s="42">
+      <c r="F45" s="27">
         <v>2</v>
       </c>
-      <c r="G45" s="44">
-        <f t="shared" ref="G45:G49" si="10">J44*$I$40</f>
+      <c r="G45" s="29">
+        <f t="shared" ref="G45:G47" si="11">J44*$I$40</f>
         <v>1441288.4499238615</v>
       </c>
-      <c r="H45" s="43">
-        <f t="shared" ref="H45:H49" si="11">$I$41</f>
+      <c r="H45" s="28">
+        <f t="shared" ref="H45:H47" si="12">$I$41</f>
         <v>10367209.879394561</v>
       </c>
-      <c r="I45" s="42">
-        <f t="shared" ref="I45:I49" si="12">H45-G45</f>
+      <c r="I45" s="27">
+        <f t="shared" ref="I45:I47" si="13">H45-G45</f>
         <v>8925921.4294706993</v>
       </c>
-      <c r="J45" s="45">
-        <f t="shared" ref="J45:J49" si="13">J44-I45</f>
+      <c r="J45" s="30">
+        <f t="shared" ref="J45:J47" si="14">J44-I45</f>
         <v>19245208.055513706</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D46" s="4"/>
-      <c r="F46" s="42">
+      <c r="D46" s="3"/>
+      <c r="F46" s="27">
         <v>3</v>
       </c>
-      <c r="G46" s="44">
-        <f t="shared" si="10"/>
+      <c r="G46" s="29">
+        <f t="shared" si="11"/>
         <v>984621.36924890568</v>
       </c>
-      <c r="H46" s="43">
-        <f t="shared" si="11"/>
+      <c r="H46" s="28">
+        <f t="shared" si="12"/>
         <v>10367209.879394561</v>
       </c>
-      <c r="I46" s="42">
-        <f t="shared" si="12"/>
+      <c r="I46" s="27">
+        <f t="shared" si="13"/>
         <v>9382588.5101456549</v>
       </c>
-      <c r="J46" s="45">
-        <f t="shared" si="13"/>
+      <c r="J46" s="30">
+        <f t="shared" si="14"/>
         <v>9862619.5453680512</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="31">
+      <c r="C47" s="52"/>
+      <c r="D47" s="53">
         <f>D44</f>
         <v>36662610.623577729</v>
       </c>
-      <c r="F47" s="46">
+      <c r="F47" s="31">
         <v>4</v>
       </c>
-      <c r="G47" s="47">
-        <f t="shared" si="10"/>
+      <c r="G47" s="32">
+        <f t="shared" si="11"/>
         <v>504590.33402650832</v>
       </c>
-      <c r="H47" s="48">
-        <f t="shared" si="11"/>
+      <c r="H47" s="33">
+        <f t="shared" si="12"/>
         <v>10367209.879394561</v>
       </c>
-      <c r="I47" s="46">
-        <f t="shared" si="12"/>
+      <c r="I47" s="31">
+        <f t="shared" si="13"/>
         <v>9862619.545368053</v>
       </c>
-      <c r="J47" s="49">
-        <f t="shared" si="13"/>
+      <c r="J47" s="34">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="7"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="41"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="54"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="25"/>
+      <c r="J48" s="26"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F49" s="38"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="41"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="25"/>
+      <c r="J49" s="26"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="30"/>
-      <c r="D50" s="28">
+      <c r="C50" s="48"/>
+      <c r="D50" s="20">
         <v>0.03</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>1</v>
       </c>
-      <c r="C53" s="13">
+      <c r="C53" s="10">
         <f>$D$15</f>
         <v>20997750.909768987</v>
       </c>
-      <c r="D53" s="13">
-        <f>-PV($D$27,B53,,C53)</f>
+      <c r="D53" s="10">
+        <f t="shared" ref="D53:D60" si="15">-PV($D$27,B53,,C53)</f>
         <v>20386165.931814551</v>
       </c>
-      <c r="F53" s="32" t="s">
+      <c r="F53" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="G53" s="32"/>
-      <c r="H53" s="33">
+      <c r="G53" s="49"/>
+      <c r="H53" s="50">
         <f>SUM(D53:D60)</f>
         <v>112289389.30267593</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>2</v>
       </c>
-      <c r="C54" s="13">
-        <f t="shared" ref="C54:C56" si="14">$D$15</f>
+      <c r="C54" s="10">
+        <f t="shared" ref="C54:C56" si="16">$D$15</f>
         <v>20997750.909768987</v>
       </c>
-      <c r="D54" s="13">
-        <f>-PV($D$27,B54,,C54)</f>
+      <c r="D54" s="10">
+        <f t="shared" si="15"/>
         <v>19792394.108557817</v>
       </c>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="34"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="51"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>3</v>
       </c>
-      <c r="C55" s="13">
-        <f t="shared" si="14"/>
+      <c r="C55" s="10">
+        <f t="shared" si="16"/>
         <v>20997750.909768987</v>
       </c>
-      <c r="D55" s="13">
-        <f>-PV($D$27,B55,,C55)</f>
+      <c r="D55" s="10">
+        <f t="shared" si="15"/>
         <v>19215916.610250305</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>4</v>
       </c>
-      <c r="C56" s="13">
-        <f t="shared" si="14"/>
+      <c r="C56" s="10">
+        <f t="shared" si="16"/>
         <v>20997750.909768987</v>
       </c>
-      <c r="D56" s="13">
-        <f>-PV($D$27,B56,,C56)</f>
+      <c r="D56" s="10">
+        <f t="shared" si="15"/>
         <v>18656229.71868962</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>5</v>
       </c>
-      <c r="C57" s="13">
+      <c r="C57" s="10">
         <f>$I$41</f>
         <v>10367209.879394561</v>
       </c>
-      <c r="D57" s="13">
-        <f>-PV($D$27,B57,,C57)</f>
+      <c r="D57" s="10">
+        <f t="shared" si="15"/>
         <v>8942846.3115200382</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>6</v>
       </c>
-      <c r="C58" s="13">
-        <f t="shared" ref="C58:C60" si="15">$I$41</f>
+      <c r="C58" s="10">
+        <f t="shared" ref="C58:C60" si="17">$I$41</f>
         <v>10367209.879394561</v>
       </c>
-      <c r="D58" s="13">
-        <f>-PV($D$27,B58,,C58)</f>
+      <c r="D58" s="10">
+        <f t="shared" si="15"/>
         <v>8682375.0597281922</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>7</v>
       </c>
-      <c r="C59" s="13">
+      <c r="C59" s="10">
+        <f t="shared" si="17"/>
+        <v>10367209.879394561</v>
+      </c>
+      <c r="D59" s="10">
         <f t="shared" si="15"/>
+        <v>8429490.3492506724</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="1">
+        <v>8</v>
+      </c>
+      <c r="C60" s="10">
+        <f t="shared" si="17"/>
         <v>10367209.879394561</v>
       </c>
-      <c r="D59" s="13">
-        <f>-PV($D$27,B59,,C59)</f>
-        <v>8429490.3492506724</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B60" s="2">
-        <v>8</v>
-      </c>
-      <c r="C60" s="13">
+      <c r="D60" s="10">
         <f t="shared" si="15"/>
-        <v>10367209.879394561</v>
-      </c>
-      <c r="D60" s="13">
-        <f>-PV($D$27,B60,,C60)</f>
         <v>8183971.2128647305</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="F53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="B47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B19:C21"/>
     <mergeCell ref="B18:C18"/>
@@ -3816,6 +3787,29 @@
     <mergeCell ref="B10:C12"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D10:D12"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="F53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="B47:C48"/>
+    <mergeCell ref="D47:D48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3825,8 +3819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54407F87-4331-4706-8B15-E2AE0F37D451}">
   <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3841,754 +3835,754 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>3</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>4</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="J8" s="5" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6">
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="61">
         <v>0.21</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
         <v>2600000</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>3400000</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <f>E9*1.08</f>
         <v>3672000.0000000005</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <f t="shared" ref="G9:H9" si="0">F9*1.08</f>
         <v>3965760.0000000009</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>4283020.8000000017</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="6"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="61"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="62">
+      <c r="C10" s="1"/>
+      <c r="D10" s="45">
         <v>8500</v>
       </c>
-      <c r="E10" s="62">
+      <c r="E10" s="45">
         <f>D10*1.035</f>
         <v>8797.5</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="45">
         <f t="shared" ref="F10:H10" si="1">E10*1.035</f>
         <v>9105.4124999999985</v>
       </c>
-      <c r="G10" s="62">
+      <c r="G10" s="45">
         <f t="shared" si="1"/>
         <v>9424.1019374999978</v>
       </c>
-      <c r="H10" s="62">
+      <c r="H10" s="45">
         <f t="shared" si="1"/>
         <v>9753.9455053124966</v>
       </c>
-      <c r="M10" s="59"/>
+      <c r="M10" s="42"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="11">
+      <c r="C11" s="1"/>
+      <c r="D11" s="8">
         <f>D9*D10</f>
         <v>22100000000</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <f t="shared" ref="E11:H11" si="2">E9*E10</f>
         <v>29911500000</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <f t="shared" si="2"/>
         <v>33435074700</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <f t="shared" si="2"/>
         <v>37373726499.660004</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="8">
         <f t="shared" si="2"/>
         <v>41776351481.319946</v>
       </c>
-      <c r="J11" s="52" t="s">
+      <c r="J11" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="44">
         <f>POWER(1+M8/2,2)-1</f>
         <v>0.22102500000000003</v>
       </c>
-      <c r="L11" s="52" t="s">
+      <c r="L11" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="M11" s="62">
+      <c r="M11" s="45">
         <f>-(C27+C28+C29+C31)*0.8</f>
         <v>16495600000</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="52"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="J12" s="52" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="J12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="62">
+      <c r="K12" s="45">
         <f>-PMT(K11,5,M11)</f>
         <v>5772992513.3477087</v>
       </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="62">
+      <c r="C14" s="1"/>
+      <c r="D14" s="45">
         <v>-120000000</v>
       </c>
-      <c r="E14" s="62">
+      <c r="E14" s="45">
         <f>D14*1.04</f>
         <v>-124800000</v>
       </c>
-      <c r="F14" s="62">
+      <c r="F14" s="45">
         <f t="shared" ref="F14:H14" si="3">E14*1.04</f>
         <v>-129792000</v>
       </c>
-      <c r="G14" s="62">
+      <c r="G14" s="45">
         <f t="shared" si="3"/>
         <v>-134983680</v>
       </c>
-      <c r="H14" s="62">
+      <c r="H14" s="45">
         <f t="shared" si="3"/>
         <v>-140383027.20000002</v>
       </c>
-      <c r="J14" s="52" t="s">
+      <c r="J14" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K14" s="52" t="s">
+      <c r="K14" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="52" t="s">
+      <c r="L14" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="M14" s="62">
+      <c r="M14" s="45">
         <f>M11</f>
         <v>16495600000</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="62">
+      <c r="C15" s="1"/>
+      <c r="D15" s="45">
         <f>-POWER(1.05,D7-1)*4500*D9-(1300000*D9/1000)-(250000*D9/1000)</f>
         <v>-15730000000</v>
       </c>
-      <c r="E15" s="62">
+      <c r="E15" s="45">
         <f t="shared" ref="E15:H15" si="4">-POWER(1.05,E7-1)*4500*E9-(1300000*E9/1000)-(250000*E9/1000)</f>
         <v>-21335000000</v>
       </c>
-      <c r="F15" s="62">
+      <c r="F15" s="45">
         <f t="shared" si="4"/>
         <v>-23909310000.000004</v>
       </c>
-      <c r="G15" s="62">
+      <c r="G15" s="45">
         <f t="shared" si="4"/>
         <v>-26805811140.000008</v>
       </c>
-      <c r="H15" s="62">
+      <c r="H15" s="45">
         <f t="shared" si="4"/>
         <v>-30065855720.76001</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="J15" s="62">
+      <c r="J15" s="45">
         <f>$K$11*M14</f>
         <v>3645939990.0000005</v>
       </c>
-      <c r="K15" s="62">
+      <c r="K15" s="45">
         <f>$K$12</f>
         <v>5772992513.3477087</v>
       </c>
-      <c r="L15" s="62">
+      <c r="L15" s="45">
         <f>K15-J15</f>
         <v>2127052523.3477082</v>
       </c>
-      <c r="M15" s="62">
+      <c r="M15" s="45">
         <f>M14-L15</f>
         <v>14368547476.652292</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <f>C29/6 + C28/12</f>
         <v>-4416666.666666667</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <f>$C$16</f>
         <v>-4416666.666666667</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="8">
         <f t="shared" ref="E16:H16" si="5">$C$16</f>
         <v>-4416666.666666667</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <f t="shared" si="5"/>
         <v>-4416666.666666667</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="8">
         <f t="shared" si="5"/>
         <v>-4416666.666666667</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="8">
         <f t="shared" si="5"/>
         <v>-4416666.666666667</v>
       </c>
       <c r="I16">
         <v>2</v>
       </c>
-      <c r="J16" s="62">
+      <c r="J16" s="45">
         <f>$K$11*M15</f>
         <v>3175808206.0270734</v>
       </c>
-      <c r="K16" s="62">
+      <c r="K16" s="45">
         <f t="shared" ref="K16:K19" si="6">$K$12</f>
         <v>5772992513.3477087</v>
       </c>
-      <c r="L16" s="62">
+      <c r="L16" s="45">
         <f t="shared" ref="L16:L19" si="7">K16-J16</f>
         <v>2597184307.3206353</v>
       </c>
-      <c r="M16" s="62">
+      <c r="M16" s="45">
         <f t="shared" ref="M16:M19" si="8">M15-L16</f>
         <v>11771363169.331657</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="62" cm="1">
+      <c r="C17" s="1"/>
+      <c r="D17" s="45" cm="1">
         <f t="array" ref="D17:H17">-TRANSPOSE(J15:J19)</f>
         <v>-3645939990.0000005</v>
       </c>
-      <c r="E17" s="62">
+      <c r="E17" s="45">
         <v>-3175808206.0270734</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="45">
         <v>-2601765544.5015297</v>
       </c>
-      <c r="G17" s="62">
+      <c r="G17" s="45">
         <v>-1900845103.7123029</v>
       </c>
-      <c r="H17" s="62">
+      <c r="H17" s="45">
         <v>-1045003722.4976373</v>
       </c>
       <c r="I17">
         <v>3</v>
       </c>
-      <c r="J17" s="62">
+      <c r="J17" s="45">
         <f>$K$11*M16</f>
         <v>2601765544.5015297</v>
       </c>
-      <c r="K17" s="62">
+      <c r="K17" s="45">
         <f t="shared" si="6"/>
         <v>5772992513.3477087</v>
       </c>
-      <c r="L17" s="62">
+      <c r="L17" s="45">
         <f t="shared" si="7"/>
         <v>3171226968.846179</v>
       </c>
-      <c r="M17" s="62">
+      <c r="M17" s="45">
         <f t="shared" si="8"/>
         <v>8600136200.4854774</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="62">
+      <c r="C18" s="1"/>
+      <c r="D18" s="45">
         <v>-7000000</v>
       </c>
-      <c r="E18" s="62">
+      <c r="E18" s="45">
         <f>D18*1.025</f>
         <v>-7174999.9999999991</v>
       </c>
-      <c r="F18" s="62">
+      <c r="F18" s="45">
         <f t="shared" ref="F18:H18" si="9">E18*1.025</f>
         <v>-7354374.9999999981</v>
       </c>
-      <c r="G18" s="62">
+      <c r="G18" s="45">
         <f t="shared" si="9"/>
         <v>-7538234.3749999972</v>
       </c>
-      <c r="H18" s="62">
+      <c r="H18" s="45">
         <f t="shared" si="9"/>
         <v>-7726690.2343749963</v>
       </c>
       <c r="I18">
         <v>4</v>
       </c>
-      <c r="J18" s="62">
+      <c r="J18" s="45">
         <f>$K$11*M17</f>
         <v>1900845103.7123029</v>
       </c>
-      <c r="K18" s="62">
+      <c r="K18" s="45">
         <f t="shared" si="6"/>
         <v>5772992513.3477087</v>
       </c>
-      <c r="L18" s="62">
+      <c r="L18" s="45">
         <f t="shared" si="7"/>
         <v>3872147409.6354055</v>
       </c>
-      <c r="M18" s="62">
+      <c r="M18" s="45">
         <f t="shared" si="8"/>
         <v>4727988790.8500719</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="11">
+      <c r="C19" s="1"/>
+      <c r="D19" s="8">
         <f>SUM(D14:D18)</f>
         <v>-19507356656.666668</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="8">
         <f t="shared" ref="E19:H19" si="10">SUM(E14:E18)</f>
         <v>-24647199872.693741</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="8">
         <f t="shared" si="10"/>
         <v>-26652638586.168201</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <f t="shared" si="10"/>
         <v>-28853594824.753979</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="8">
         <f t="shared" si="10"/>
         <v>-31263385827.358692</v>
       </c>
       <c r="I19">
         <v>5</v>
       </c>
-      <c r="J19" s="62">
+      <c r="J19" s="45">
         <f>$K$11*M18</f>
         <v>1045003722.4976373</v>
       </c>
-      <c r="K19" s="62">
+      <c r="K19" s="45">
         <f t="shared" si="6"/>
         <v>5772992513.3477087</v>
       </c>
-      <c r="L19" s="62">
+      <c r="L19" s="45">
         <f t="shared" si="7"/>
         <v>4727988790.850071</v>
       </c>
-      <c r="M19" s="62">
+      <c r="M19" s="45">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="11">
+      <c r="C20" s="1"/>
+      <c r="D20" s="8">
         <f>D11+D19</f>
         <v>2592643343.3333321</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="8">
         <f t="shared" ref="E20:H20" si="11">E11+E19</f>
         <v>5264300127.3062592</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8">
         <f t="shared" si="11"/>
         <v>6782436113.8317986</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="8">
         <f t="shared" si="11"/>
         <v>8520131674.9060249</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="8">
         <f t="shared" si="11"/>
         <v>10512965653.961254</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="60">
+      <c r="C21" s="43">
         <v>-0.27</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="45">
         <f>D20*$C$21</f>
         <v>-700013702.69999969</v>
       </c>
-      <c r="E21" s="62">
+      <c r="E21" s="45">
         <f>E20*$C$21</f>
         <v>-1421361034.37269</v>
       </c>
-      <c r="F21" s="62">
-        <f t="shared" ref="E21:H21" si="12">F20*$C$21</f>
+      <c r="F21" s="45">
+        <f t="shared" ref="F21:H21" si="12">F20*$C$21</f>
         <v>-1831257750.7345858</v>
       </c>
-      <c r="G21" s="62">
+      <c r="G21" s="45">
         <f t="shared" si="12"/>
         <v>-2300435552.224627</v>
       </c>
-      <c r="H21" s="62">
+      <c r="H21" s="45">
         <f t="shared" si="12"/>
         <v>-2838500726.5695386</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="52"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="62">
+      <c r="C23" s="1"/>
+      <c r="D23" s="45">
         <f>D20+D21</f>
         <v>1892629640.6333323</v>
       </c>
-      <c r="E23" s="62">
+      <c r="E23" s="45">
         <f t="shared" ref="E23:H23" si="13">E20+E21</f>
         <v>3842939092.933569</v>
       </c>
-      <c r="F23" s="62">
+      <c r="F23" s="45">
         <f t="shared" si="13"/>
         <v>4951178363.0972128</v>
       </c>
-      <c r="G23" s="62">
+      <c r="G23" s="45">
         <f t="shared" si="13"/>
         <v>6219696122.6813984</v>
       </c>
-      <c r="H23" s="62">
+      <c r="H23" s="45">
         <f t="shared" si="13"/>
         <v>7674464927.391716</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="11">
+      <c r="C24" s="1"/>
+      <c r="D24" s="8">
         <f>-D16</f>
         <v>4416666.666666667</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="8">
         <f t="shared" ref="E24:H24" si="14">-E16</f>
         <v>4416666.666666667</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="8">
         <f t="shared" si="14"/>
         <v>4416666.666666667</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="8">
         <f t="shared" si="14"/>
         <v>4416666.666666667</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="8">
         <f t="shared" si="14"/>
         <v>4416666.666666667</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="62" cm="1">
+      <c r="C25" s="1"/>
+      <c r="D25" s="45" cm="1">
         <f t="array" ref="D25:H25">-TRANSPOSE(L15:L19)</f>
         <v>-2127052523.3477082</v>
       </c>
-      <c r="E25" s="62">
+      <c r="E25" s="45">
         <v>-2597184307.3206353</v>
       </c>
-      <c r="F25" s="62">
+      <c r="F25" s="45">
         <v>-3171226968.846179</v>
       </c>
-      <c r="G25" s="62">
+      <c r="G25" s="45">
         <v>-3872147409.6354055</v>
       </c>
-      <c r="H25" s="62">
+      <c r="H25" s="45">
         <v>-4727988790.850071</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="62">
+      <c r="C27" s="45">
         <v>-130000000</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="62">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="45">
         <f>(-C27)*0.7</f>
         <v>91000000</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="62">
+      <c r="C28" s="45">
         <v>-28000000</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="62">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="45">
         <f>-(C28+C28/12)*0.7</f>
         <v>21233333.333333332</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="62">
+      <c r="C29" s="45">
         <v>-12500000</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="62">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="45">
         <f>-(C29+C29/6)*0.7</f>
         <v>10208333.333333334</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="52">
+      <c r="C30" s="37">
         <f>M14</f>
         <v>16495600000</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="52" t="s">
+      <c r="B31" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="8">
         <f>1.3*D15</f>
         <v>-20449000000</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="11">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="8">
         <f>-0.85*C31</f>
         <v>17381650000</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="62">
+      <c r="C32" s="45">
         <f>SUM(C23:C31)</f>
         <v>-4123900000</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="45">
         <f t="shared" ref="D32:H32" si="15">SUM(D23:D31)</f>
         <v>-230006216.04770923</v>
       </c>
-      <c r="E32" s="62">
+      <c r="E32" s="45">
         <f t="shared" si="15"/>
         <v>1250171452.2796001</v>
       </c>
-      <c r="F32" s="62">
+      <c r="F32" s="45">
         <f t="shared" si="15"/>
         <v>1784368060.9177008</v>
       </c>
-      <c r="G32" s="62">
+      <c r="G32" s="45">
         <f t="shared" si="15"/>
         <v>2351965379.7126598</v>
       </c>
-      <c r="H32" s="62">
+      <c r="H32" s="45">
         <f t="shared" si="15"/>
         <v>20454984469.874977</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="63">
+      <c r="C33" s="46">
         <f>3%+1.25*11%</f>
         <v>0.16750000000000001</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="10">
         <f>NPV(C33,D32:H32)+C32</f>
         <v>8413531372.3701782</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="28">
+      <c r="C35" s="20">
         <f>IRR(C32:H32)</f>
         <v>0.49710654925254549</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4620,69 +4614,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="G3" s="3"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>2000</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>10</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="38" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>2000</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>40</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="38" t="s">
         <v>3</v>
       </c>
       <c r="F7" t="s">
@@ -4696,869 +4690,869 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>2001</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>30</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="39">
         <v>2000</v>
       </c>
-      <c r="F8" s="55">
+      <c r="F8">
         <v>10</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8">
         <v>40</v>
       </c>
-      <c r="H8" s="55">
+      <c r="H8">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>2001</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>57</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="39">
         <v>2001</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9">
         <v>30</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9">
         <v>57</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9">
         <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>2002</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>48</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="39">
         <v>2002</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10">
         <v>48</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10">
         <v>68</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H10">
         <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>2002</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>68</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="39">
         <v>2003</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11">
         <v>64</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11">
         <v>120</v>
       </c>
-      <c r="H11" s="55">
+      <c r="H11">
         <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>2003</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>64</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="39">
         <v>2004</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12">
         <v>78</v>
       </c>
-      <c r="G12" s="55">
+      <c r="G12">
         <v>180</v>
       </c>
-      <c r="H12" s="55">
+      <c r="H12">
         <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>2003</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>120</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="39">
         <v>2005</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13">
         <v>90</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13">
         <v>230</v>
       </c>
-      <c r="H13" s="55">
+      <c r="H13">
         <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>2004</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>78</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="39">
         <v>2006</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14">
         <v>100</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14">
         <v>320</v>
       </c>
-      <c r="H14" s="55">
+      <c r="H14">
         <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>2004</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>180</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="39">
         <v>2007</v>
       </c>
-      <c r="F15" s="55">
+      <c r="F15">
         <v>109</v>
       </c>
-      <c r="G15" s="55">
+      <c r="G15">
         <v>390</v>
       </c>
-      <c r="H15" s="55">
+      <c r="H15">
         <v>499</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>2005</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>90</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="39">
         <v>2008</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16">
         <v>114</v>
       </c>
-      <c r="G16" s="55">
+      <c r="G16">
         <v>450</v>
       </c>
-      <c r="H16" s="55">
+      <c r="H16">
         <v>564</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>2005</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>230</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="39">
         <v>2009</v>
       </c>
-      <c r="F17" s="55">
+      <c r="F17">
         <v>117</v>
       </c>
-      <c r="G17" s="55">
+      <c r="G17">
         <v>540</v>
       </c>
-      <c r="H17" s="55">
+      <c r="H17">
         <v>657</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>2006</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>100</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="39">
         <v>2010</v>
       </c>
-      <c r="F18" s="55">
+      <c r="F18">
         <v>118</v>
       </c>
-      <c r="G18" s="55">
+      <c r="G18">
         <v>590</v>
       </c>
-      <c r="H18" s="55">
+      <c r="H18">
         <v>708</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>2006</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>320</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="39">
         <v>2011</v>
       </c>
-      <c r="F19" s="55">
+      <c r="F19">
         <v>118</v>
       </c>
-      <c r="G19" s="55">
+      <c r="G19">
         <v>760</v>
       </c>
-      <c r="H19" s="55">
+      <c r="H19">
         <v>878</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>2007</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>109</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="39">
         <v>2012</v>
       </c>
-      <c r="F20" s="55">
+      <c r="F20">
         <v>119</v>
       </c>
-      <c r="G20" s="55">
+      <c r="G20">
         <v>960</v>
       </c>
-      <c r="H20" s="55">
+      <c r="H20">
         <v>1079</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>2007</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>390</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="39">
         <v>2013</v>
       </c>
-      <c r="F21" s="55">
+      <c r="F21">
         <v>123</v>
       </c>
-      <c r="G21" s="55">
+      <c r="G21">
         <v>1100</v>
       </c>
-      <c r="H21" s="55">
+      <c r="H21">
         <v>1223</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>2008</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>114</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="39">
         <v>2014</v>
       </c>
-      <c r="F22" s="55">
+      <c r="F22">
         <v>128</v>
       </c>
-      <c r="G22" s="55">
+      <c r="G22">
         <v>1500</v>
       </c>
-      <c r="H22" s="55">
+      <c r="H22">
         <v>1628</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>2008</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>450</v>
       </c>
-      <c r="E23" s="54">
+      <c r="E23" s="39">
         <v>2015</v>
       </c>
-      <c r="F23" s="55">
+      <c r="F23">
         <v>134</v>
       </c>
-      <c r="G23" s="55">
+      <c r="G23">
         <v>2000</v>
       </c>
-      <c r="H23" s="55">
+      <c r="H23">
         <v>2134</v>
       </c>
-      <c r="J23" s="57" t="s">
+      <c r="J23" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="L23" s="57" t="s">
+      <c r="L23" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="M23" s="57" t="s">
+      <c r="M23" s="22" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>2009</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>117</v>
       </c>
-      <c r="E24" s="54">
+      <c r="E24" s="39">
         <v>2016</v>
       </c>
-      <c r="F24" s="55">
+      <c r="F24">
         <v>137</v>
       </c>
-      <c r="G24" s="55">
+      <c r="G24">
         <v>2600</v>
       </c>
-      <c r="H24" s="55">
+      <c r="H24">
         <v>2737</v>
       </c>
-      <c r="J24" s="57" t="s">
+      <c r="J24" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="58" t="s">
+      <c r="K24" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="L24" s="57" t="s">
+      <c r="L24" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="M24" s="57" t="s">
+      <c r="M24" s="22" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>2009</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>540</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="39">
         <v>2017</v>
       </c>
-      <c r="F25" s="55">
+      <c r="F25">
         <v>137</v>
       </c>
-      <c r="G25" s="55">
+      <c r="G25">
         <v>3500</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H25">
         <v>3637</v>
       </c>
-      <c r="J25" s="57" t="s">
+      <c r="J25" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="58" t="s">
+      <c r="K25" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="L25" s="57" t="s">
+      <c r="L25" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="M25" s="57" t="s">
+      <c r="M25" s="22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>2010</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>118</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E26" s="39">
         <v>2018</v>
       </c>
-      <c r="F26" s="55">
+      <c r="F26">
         <v>140</v>
       </c>
-      <c r="G26" s="55">
+      <c r="G26">
         <v>4600</v>
       </c>
-      <c r="H26" s="55">
+      <c r="H26">
         <v>4740</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>2010</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>590</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="39">
         <v>2019</v>
       </c>
-      <c r="F27" s="55">
+      <c r="F27">
         <v>145</v>
       </c>
-      <c r="G27" s="55">
+      <c r="G27">
         <v>5400</v>
       </c>
-      <c r="H27" s="55">
+      <c r="H27">
         <v>5545</v>
       </c>
-      <c r="L27" s="56"/>
+      <c r="L27" s="40"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>2011</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>118</v>
       </c>
-      <c r="E28" s="54">
+      <c r="E28" s="39">
         <v>2020</v>
       </c>
-      <c r="F28" s="55">
+      <c r="F28">
         <v>150</v>
       </c>
-      <c r="G28" s="55">
+      <c r="G28">
         <v>6700</v>
       </c>
-      <c r="H28" s="55">
+      <c r="H28">
         <v>6850</v>
       </c>
-      <c r="L28" s="56"/>
+      <c r="L28" s="40"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>2011</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>760</v>
       </c>
-      <c r="E29" s="54">
+      <c r="E29" s="39">
         <v>2021</v>
       </c>
-      <c r="F29" s="55">
+      <c r="F29">
         <v>152</v>
       </c>
-      <c r="G29" s="55">
+      <c r="G29">
         <v>7200</v>
       </c>
-      <c r="H29" s="55">
+      <c r="H29">
         <v>7352</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>2012</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>119</v>
       </c>
-      <c r="E30" s="54">
+      <c r="E30" s="39">
         <v>2022</v>
       </c>
-      <c r="F30" s="55">
+      <c r="F30">
         <v>155</v>
       </c>
-      <c r="G30" s="55">
+      <c r="G30">
         <v>7900</v>
       </c>
-      <c r="H30" s="55">
+      <c r="H30">
         <v>8055</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>2012</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>960</v>
       </c>
-      <c r="E31" s="54">
+      <c r="E31" s="39">
         <v>2023</v>
       </c>
-      <c r="F31" s="55">
+      <c r="F31">
         <v>157</v>
       </c>
-      <c r="G31" s="55">
+      <c r="G31">
         <v>8200</v>
       </c>
-      <c r="H31" s="55">
+      <c r="H31">
         <v>8357</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>2013</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>123</v>
       </c>
-      <c r="E32" s="54">
+      <c r="E32" s="39">
         <v>2024</v>
       </c>
-      <c r="F32" s="55">
+      <c r="F32">
         <v>158</v>
       </c>
-      <c r="G32" s="55">
+      <c r="G32">
         <v>8500</v>
       </c>
-      <c r="H32" s="55">
+      <c r="H32">
         <v>8658</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>2013</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>1100</v>
       </c>
-      <c r="E33" s="54" t="s">
+      <c r="E33" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="55">
+      <c r="F33">
         <v>2831</v>
       </c>
-      <c r="G33" s="55">
+      <c r="G33">
         <v>63905</v>
       </c>
-      <c r="H33" s="55">
+      <c r="H33">
         <v>66736</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>2014</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>2014</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>1500</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>2015</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>2015</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>2000</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>2016</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>2016</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>2600</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>2017</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>2017</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>3500</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>2018</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>2018</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>4600</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>2019</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>2019</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>5400</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>2020</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>2020</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>6700</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>2021</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>2021</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>7200</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>2022</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>2022</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>7900</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>2023</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>2023</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>8200</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>2024</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>158</v>
       </c>
       <c r="E54" t="s">
@@ -5569,13 +5563,13 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>2024</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>8500</v>
       </c>
       <c r="E55" t="s">

</xml_diff>